<commit_message>
some more documentation tags, updated mapping for CSV and Facebook connectors
</commit_message>
<xml_diff>
--- a/SemSync-Mapping.xlsx
+++ b/SemSync-Mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
   <si>
     <t>Outlook</t>
   </si>
@@ -386,6 +386,54 @@
   </si>
   <si>
     <t>info</t>
+  </si>
+  <si>
+    <t>Csv</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentCountryName</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentCityName</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentPostalCode</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentStreetName</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentRoom</t>
+  </si>
+  <si>
+    <t>BusinessDepartmentPhone</t>
+  </si>
+  <si>
+    <t>ProfileUpdateDate</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>HometownLocation.Country</t>
+  </si>
+  <si>
+    <t>HometownLocation.State</t>
+  </si>
+  <si>
+    <t>HometownLocation.City</t>
+  </si>
+  <si>
+    <t>HometownLocation.ZipCode</t>
+  </si>
+  <si>
+    <t>PictureBigBytes</t>
+  </si>
+  <si>
+    <t>UserId</t>
   </si>
 </sst>
 </file>
@@ -841,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,46 +976,58 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1264,10 +1324,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1275,16 +1338,18 @@
     <col min="1" max="1" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="26.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:10" s="22" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1294,80 +1359,89 @@
       <c r="F1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="43" t="s">
         <v>94</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="35"/>
-      <c r="B3" s="38"/>
+      <c r="G2" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="36"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="35"/>
-      <c r="B4" s="38"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="36"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="35"/>
-      <c r="B5" s="38"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="36"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="35"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="36"/>
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
@@ -1375,18 +1449,21 @@
       <c r="D6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>91</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="35"/>
+      <c r="G6" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="36"/>
       <c r="B7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1394,16 +1471,19 @@
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="35"/>
+      <c r="G7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="36"/>
       <c r="B8" s="7" t="s">
         <v>45</v>
       </c>
@@ -1415,12 +1495,15 @@
       <c r="F8" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="35"/>
+      <c r="G8" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="45"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="36"/>
       <c r="B9" s="7" t="s">
         <v>46</v>
       </c>
@@ -1430,12 +1513,15 @@
       <c r="F9" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="35"/>
+      <c r="G9" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="36"/>
       <c r="B10" s="7" t="s">
         <v>47</v>
       </c>
@@ -1443,48 +1529,53 @@
       <c r="D10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="35"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="36"/>
       <c r="B11" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="35"/>
+      <c r="G11" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="45"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="31"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="35"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="36"/>
       <c r="B13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1492,15 +1583,16 @@
       <c r="D13" s="33"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="35" t="s">
+      <c r="G13" s="46"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1509,51 +1601,55 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="35"/>
-      <c r="B15" s="38"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="36"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="35"/>
-      <c r="B16" s="38"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="36"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="35"/>
-      <c r="B17" s="38"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="36"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="35"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="36"/>
       <c r="B18" s="7" t="s">
         <v>43</v>
       </c>
@@ -1561,12 +1657,13 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="35"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="36"/>
       <c r="B19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1574,12 +1671,13 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="35"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
@@ -1587,12 +1685,13 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="35"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="36"/>
       <c r="B21" s="7" t="s">
         <v>46</v>
       </c>
@@ -1600,12 +1699,13 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="35"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="36"/>
       <c r="B22" s="7" t="s">
         <v>47</v>
       </c>
@@ -1613,12 +1713,13 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="35"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="36"/>
       <c r="B23" s="7" t="s">
         <v>48</v>
       </c>
@@ -1626,12 +1727,13 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="35"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
         <v>72</v>
       </c>
@@ -1639,12 +1741,13 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="35"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="36"/>
       <c r="B25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1652,74 +1755,79 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="35" t="s">
+      <c r="G25" s="46"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="35"/>
-      <c r="B27" s="38"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="36"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="35"/>
-      <c r="B28" s="38"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="36"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="35"/>
-      <c r="B29" s="38"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="36"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="33"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="35"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="36"/>
       <c r="B30" s="7" t="s">
         <v>43</v>
       </c>
@@ -1727,16 +1835,19 @@
       <c r="D30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="31" t="s">
         <v>92</v>
       </c>
       <c r="F30" s="11"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="35"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="36"/>
       <c r="B31" s="7" t="s">
         <v>44</v>
       </c>
@@ -1744,14 +1855,17 @@
       <c r="D31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="11"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="35"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="36"/>
       <c r="B32" s="7" t="s">
         <v>45</v>
       </c>
@@ -1761,12 +1875,15 @@
       </c>
       <c r="E32" s="33"/>
       <c r="F32" s="11"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="35"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="36"/>
       <c r="B33" s="7" t="s">
         <v>46</v>
       </c>
@@ -1774,12 +1891,13 @@
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="35"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="36"/>
       <c r="B34" s="7" t="s">
         <v>47</v>
       </c>
@@ -1787,44 +1905,49 @@
       <c r="D34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="32" t="s">
         <v>92</v>
       </c>
       <c r="F34" s="11"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="35"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="36"/>
       <c r="B35" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="35"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="36"/>
       <c r="B36" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C36" s="18"/>
-      <c r="D36" s="31"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="35"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="36"/>
       <c r="B37" s="7" t="s">
         <v>49</v>
       </c>
@@ -1832,15 +1955,16 @@
       <c r="D37" s="33"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="35" t="s">
+      <c r="G37" s="46"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1849,51 +1973,55 @@
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="35"/>
-      <c r="B39" s="38"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="36"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="35"/>
-      <c r="B40" s="38"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="36"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="35"/>
-      <c r="B41" s="38"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="36"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="35"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="36"/>
       <c r="B42" s="7" t="s">
         <v>43</v>
       </c>
@@ -1901,12 +2029,13 @@
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="35"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="36"/>
       <c r="B43" s="7" t="s">
         <v>44</v>
       </c>
@@ -1914,12 +2043,13 @@
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="35"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="36"/>
       <c r="B44" s="7" t="s">
         <v>45</v>
       </c>
@@ -1927,12 +2057,13 @@
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="35"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="36"/>
       <c r="B45" s="7" t="s">
         <v>46</v>
       </c>
@@ -1940,12 +2071,13 @@
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="35"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="36"/>
       <c r="B46" s="7" t="s">
         <v>47</v>
       </c>
@@ -1953,12 +2085,13 @@
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="35"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="36"/>
       <c r="B47" s="7" t="s">
         <v>48</v>
       </c>
@@ -1966,12 +2099,13 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="35"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="36"/>
       <c r="B48" s="7" t="s">
         <v>72</v>
       </c>
@@ -1979,12 +2113,13 @@
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="35"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="36"/>
       <c r="B49" s="4" t="s">
         <v>49</v>
       </c>
@@ -1992,12 +2127,13 @@
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="35" t="s">
+      <c r="G49" s="46"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -2007,12 +2143,13 @@
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="11"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="35"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="36"/>
       <c r="B51" s="7" t="s">
         <v>8</v>
       </c>
@@ -2020,12 +2157,13 @@
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="35"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="36"/>
       <c r="B52" s="7" t="s">
         <v>9</v>
       </c>
@@ -2033,12 +2171,13 @@
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="35"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="36"/>
       <c r="B53" s="7" t="s">
         <v>10</v>
       </c>
@@ -2046,55 +2185,59 @@
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="35" t="s">
+      <c r="G53" s="46"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="32" t="s">
+      <c r="D54" s="31" t="s">
         <v>67</v>
       </c>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="35"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="36"/>
       <c r="B55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="18"/>
-      <c r="D55" s="31"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="35"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="36"/>
       <c r="B56" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="18"/>
-      <c r="D56" s="31"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="35"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="36"/>
       <c r="B57" s="7" t="s">
         <v>10</v>
       </c>
@@ -2102,12 +2245,13 @@
       <c r="D57" s="33"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="35" t="s">
+      <c r="G57" s="46"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="36" t="s">
         <v>22</v>
       </c>
       <c r="B58" s="7" t="s">
@@ -2117,16 +2261,17 @@
       <c r="D58" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E58" s="32" t="s">
         <v>87</v>
       </c>
       <c r="F58" s="11"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="35"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="36"/>
       <c r="B59" s="7" t="s">
         <v>12</v>
       </c>
@@ -2134,16 +2279,21 @@
       <c r="D59" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="31"/>
+      <c r="E59" s="32"/>
       <c r="F59" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="3"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="35"/>
+      <c r="G59" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I59" s="5"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="36"/>
       <c r="B60" s="7" t="s">
         <v>13</v>
       </c>
@@ -2151,14 +2301,17 @@
       <c r="D60" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="31"/>
+      <c r="E60" s="32"/>
       <c r="F60" s="11"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="3"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="35"/>
+      <c r="G60" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="45"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="36"/>
       <c r="B61" s="7" t="s">
         <v>14</v>
       </c>
@@ -2166,16 +2319,21 @@
       <c r="D61" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="32"/>
       <c r="F61" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="35"/>
+      <c r="G61" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="36"/>
       <c r="B62" s="7" t="s">
         <v>15</v>
       </c>
@@ -2183,12 +2341,13 @@
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="35"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="36"/>
       <c r="B63" s="7" t="s">
         <v>16</v>
       </c>
@@ -2196,12 +2355,13 @@
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="3"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="35"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="36"/>
       <c r="B64" s="7" t="s">
         <v>17</v>
       </c>
@@ -2209,117 +2369,127 @@
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="35" t="s">
+      <c r="G64" s="46"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="12"/>
-      <c r="D65" s="32" t="s">
+      <c r="D65" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="E65" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="F65" s="34" t="s">
+      <c r="F65" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="35"/>
+      <c r="G65" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H65" s="45"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="36"/>
       <c r="B66" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C66" s="18"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="31"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="35"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="36"/>
       <c r="B67" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="18"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="35"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="36"/>
       <c r="B68" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="33"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="35" t="s">
+      <c r="E68" s="32"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="12"/>
-      <c r="D69" s="32" t="s">
+      <c r="D69" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E69" s="32" t="s">
+      <c r="E69" s="31" t="s">
         <v>95</v>
       </c>
       <c r="F69" s="11"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="35"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="36"/>
       <c r="B70" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C70" s="18"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
       <c r="F70" s="11"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="35"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="45"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="36"/>
       <c r="B71" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C71" s="18"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
       <c r="F71" s="11"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="35"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="36"/>
       <c r="B72" s="7" t="s">
         <v>6</v>
       </c>
@@ -2327,12 +2497,13 @@
       <c r="D72" s="33"/>
       <c r="E72" s="33"/>
       <c r="F72" s="11"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="35" t="s">
+      <c r="G72" s="46"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="7" t="s">
@@ -2342,12 +2513,13 @@
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="35"/>
+      <c r="G73" s="46"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="36"/>
       <c r="B74" s="7" t="s">
         <v>18</v>
       </c>
@@ -2355,12 +2527,15 @@
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="35"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="36"/>
       <c r="B75" s="7" t="s">
         <v>19</v>
       </c>
@@ -2368,11 +2543,14 @@
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="G75" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="45"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="16" t="s">
         <v>21</v>
       </c>
@@ -2384,11 +2562,14 @@
         <v>101</v>
       </c>
       <c r="F76" s="11"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="G76" s="46"/>
+      <c r="H76" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="14" t="s">
         <v>122</v>
       </c>
@@ -2400,11 +2581,14 @@
         <v>90</v>
       </c>
       <c r="F77" s="11"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="G77" s="46"/>
+      <c r="H77" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="14" t="s">
         <v>121</v>
       </c>
@@ -2416,11 +2600,16 @@
       <c r="F78" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G78" s="2"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="G78" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="14" t="s">
         <v>54</v>
       </c>
@@ -2434,11 +2623,14 @@
       <c r="F79" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="G79" s="2"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="G79" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H79" s="45"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="14" t="s">
         <v>57</v>
       </c>
@@ -2452,11 +2644,14 @@
       <c r="F80" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="G80" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H80" s="45"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="14" t="s">
         <v>58</v>
       </c>
@@ -2466,11 +2661,14 @@
       <c r="F81" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="G81" s="2"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="G81" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H81" s="45"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="14" t="s">
         <v>59</v>
       </c>
@@ -2484,11 +2682,14 @@
       <c r="F82" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="G82" s="2"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="G82" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H82" s="45"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="14" t="s">
         <v>60</v>
       </c>
@@ -2496,11 +2697,12 @@
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="G83" s="46"/>
+      <c r="H83" s="45"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="14" t="s">
         <v>61</v>
       </c>
@@ -2512,11 +2714,12 @@
         <v>98</v>
       </c>
       <c r="F84" s="11"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="G84" s="46"/>
+      <c r="H84" s="45"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="14" t="s">
         <v>62</v>
       </c>
@@ -2530,11 +2733,12 @@
       <c r="F85" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="G85" s="46"/>
+      <c r="H85" s="45"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="14" t="s">
         <v>63</v>
       </c>
@@ -2546,11 +2750,12 @@
         <v>88</v>
       </c>
       <c r="F86" s="11"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="G86" s="46"/>
+      <c r="H86" s="45"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="14" t="s">
         <v>64</v>
       </c>
@@ -2558,11 +2763,12 @@
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="G87" s="46"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="14" t="s">
         <v>65</v>
       </c>
@@ -2574,11 +2780,12 @@
         <v>89</v>
       </c>
       <c r="F88" s="11"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="G88" s="46"/>
+      <c r="H88" s="45"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="17" t="s">
         <v>66</v>
       </c>
@@ -2588,12 +2795,13 @@
       </c>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="39" t="s">
+      <c r="G89" s="46"/>
+      <c r="H89" s="45"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B90" s="7" t="s">
@@ -2607,12 +2815,15 @@
       <c r="F90" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G90" s="2"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A91" s="40"/>
+      <c r="G90" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90" s="45"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A91" s="35"/>
       <c r="B91" s="15" t="s">
         <v>25</v>
       </c>
@@ -2624,15 +2835,41 @@
       <c r="F91" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G91" s="26"/>
-      <c r="H91" s="28"/>
-      <c r="I91" s="27"/>
+      <c r="G91" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H91" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="I91" s="28"/>
+      <c r="J91" s="27"/>
     </row>
   </sheetData>
   <sortState ref="A2:A53">
     <sortCondition ref="A53"/>
   </sortState>
-  <mergeCells count="35">
+  <mergeCells count="37">
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G65:G68"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B29"/>
     <mergeCell ref="D65:D68"/>
     <mergeCell ref="A90:A91"/>
     <mergeCell ref="A69:A72"/>
@@ -2649,25 +2886,6 @@
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E26:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add Mapping information LotusNotes start write to LotusNotes
</commit_message>
<xml_diff>
--- a/SemSync-Mapping.xlsx
+++ b/SemSync-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="22455" windowHeight="11475"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping of StdContact" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="158">
   <si>
     <t>Outlook</t>
   </si>
@@ -436,7 +436,58 @@
     <t>UserId</t>
   </si>
   <si>
-    <t>not implemented yet</t>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>InternetAddress</t>
+  </si>
+  <si>
+    <t>OfficePhoneNumber</t>
+  </si>
+  <si>
+    <t>OfficeStreetAddress</t>
+  </si>
+  <si>
+    <t>OfficeState</t>
+  </si>
+  <si>
+    <t>OfficeCity</t>
+  </si>
+  <si>
+    <t>OfficeZIP</t>
+  </si>
+  <si>
+    <t>OfficeCountry</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StreetAddress </t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>CellPhoneNumber</t>
   </si>
 </sst>
 </file>
@@ -480,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -810,13 +861,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -826,10 +877,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -839,21 +890,8 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -865,11 +903,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -878,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,9 +984,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,6 +996,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -968,66 +1017,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1035,9 +1081,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1075,7 +1121,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1145,7 +1191,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1322,13 +1368,13 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J92" sqref="J92"/>
+      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -1338,22 +1384,22 @@
     <col min="7" max="7" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="29" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="22" t="s">
@@ -1365,84 +1411,84 @@
       <c r="I1" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="42" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>130</v>
       </c>
       <c r="H2" s="19"/>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="47" t="s">
-        <v>140</v>
+      <c r="J2" s="49" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="32"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="48"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="47"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="48"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="32"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="31"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="48"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="6" t="s">
         <v>43</v>
       </c>
@@ -1450,23 +1496,25 @@
       <c r="D6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="32" t="s">
         <v>91</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>126</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="48"/>
+      <c r="J6" s="50" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="32"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="6" t="s">
         <v>44</v>
       </c>
@@ -1474,19 +1522,21 @@
       <c r="D7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>125</v>
       </c>
       <c r="H7" s="10"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="48"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="50" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="32"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="6" t="s">
         <v>45</v>
       </c>
@@ -1494,19 +1544,21 @@
       <c r="D8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>127</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="48"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="50" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="32"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="6" t="s">
         <v>46</v>
       </c>
@@ -1516,15 +1568,15 @@
       <c r="F9" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
         <v>129</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="48"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="6" t="s">
         <v>47</v>
       </c>
@@ -1532,7 +1584,7 @@
       <c r="D10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="31" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="13" t="s">
@@ -1540,64 +1592,68 @@
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="48"/>
+      <c r="J10" s="50" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="32"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
         <v>128</v>
       </c>
       <c r="H11" s="10"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="48"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="50" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="32"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="28"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="43"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="48"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="32"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="43"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="48"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1605,236 +1661,238 @@
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="43"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="48"/>
+      <c r="J14" s="47"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="32"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="43"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="48"/>
+      <c r="J15" s="47"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="32"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="43"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="48"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="32"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="43"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="48"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="32"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="43"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="48"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="32"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="43"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="48"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="32"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="43"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="48"/>
+      <c r="J20" s="47"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="32"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="43"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="48"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="32"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="43"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="48"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="32"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="43"/>
+      <c r="F23" s="27"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="48"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="32"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="43"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="48"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="32"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="43"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="48"/>
+      <c r="J25" s="47"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="45" t="s">
         <v>117</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="29" t="s">
+      <c r="I26" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="48"/>
+      <c r="J26" s="50" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="32"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="42"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="48"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="51"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="32"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="42"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="48"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="47"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="32"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="42"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="48"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="32"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="6" t="s">
         <v>43</v>
       </c>
@@ -1842,21 +1900,23 @@
       <c r="D30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="43"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="27" t="s">
+      <c r="H30" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="I30" s="29" t="s">
+      <c r="I30" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="J30" s="48"/>
+      <c r="J30" s="50" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="32"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
@@ -1864,17 +1924,19 @@
       <c r="D31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="43"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="27" t="s">
+      <c r="H31" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="J31" s="48"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="50" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="32"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="6" t="s">
         <v>45</v>
       </c>
@@ -1882,31 +1944,33 @@
       <c r="D32" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="43"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="27" t="s">
+      <c r="H32" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="48"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="50" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="32"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="43"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
-      <c r="J33" s="48"/>
+      <c r="J33" s="47"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="32"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="6" t="s">
         <v>47</v>
       </c>
@@ -1914,68 +1978,72 @@
       <c r="D34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="27" t="s">
+      <c r="H34" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J34" s="48"/>
+      <c r="J34" s="50" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="32"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="17"/>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="48"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="50" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="32"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="28"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="10"/>
-      <c r="F36" s="43"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
-      <c r="J36" s="48"/>
+      <c r="J36" s="47"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="32"/>
+      <c r="A37" s="36"/>
       <c r="B37" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="30"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="43"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="48"/>
+      <c r="J37" s="47"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="40" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -1983,168 +2051,168 @@
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
-      <c r="F38" s="43"/>
+      <c r="F38" s="27"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
-      <c r="J38" s="48"/>
+      <c r="J38" s="47"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="32"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
-      <c r="F39" s="43"/>
+      <c r="F39" s="27"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
-      <c r="J39" s="48"/>
+      <c r="J39" s="47"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="32"/>
-      <c r="B40" s="35"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="43"/>
+      <c r="F40" s="27"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
-      <c r="J40" s="48"/>
+      <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="32"/>
-      <c r="B41" s="35"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
-      <c r="F41" s="43"/>
+      <c r="F41" s="27"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="48"/>
+      <c r="J41" s="47"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="32"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="43"/>
+      <c r="F42" s="27"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="48"/>
+      <c r="J42" s="47"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="32"/>
+      <c r="A43" s="36"/>
       <c r="B43" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
-      <c r="F43" s="43"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
-      <c r="J43" s="48"/>
+      <c r="J43" s="47"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="32"/>
+      <c r="A44" s="36"/>
       <c r="B44" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="43"/>
+      <c r="F44" s="27"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
-      <c r="J44" s="48"/>
+      <c r="J44" s="47"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="32"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
-      <c r="F45" s="43"/>
+      <c r="F45" s="27"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
-      <c r="J45" s="48"/>
+      <c r="J45" s="47"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="32"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
-      <c r="F46" s="43"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
-      <c r="J46" s="48"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="32"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
-      <c r="F47" s="43"/>
+      <c r="F47" s="27"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="48"/>
+      <c r="J47" s="47"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="32"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="43"/>
+      <c r="F48" s="27"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
-      <c r="J48" s="48"/>
+      <c r="J48" s="47"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="32"/>
+      <c r="A49" s="36"/>
       <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
-      <c r="F49" s="43"/>
+      <c r="F49" s="27"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
-      <c r="J49" s="48"/>
+      <c r="J49" s="47"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -2153,116 +2221,116 @@
       <c r="C50" s="11"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19"/>
-      <c r="F50" s="43"/>
+      <c r="F50" s="27"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
       <c r="I50" s="19"/>
-      <c r="J50" s="48"/>
+      <c r="J50" s="47"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="32"/>
+      <c r="A51" s="36"/>
       <c r="B51" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
-      <c r="F51" s="43"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
-      <c r="J51" s="48"/>
+      <c r="J51" s="47"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="32"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="17"/>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
-      <c r="F52" s="43"/>
+      <c r="F52" s="27"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
-      <c r="J52" s="48"/>
+      <c r="J52" s="47"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="32"/>
+      <c r="A53" s="36"/>
       <c r="B53" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
-      <c r="F53" s="43"/>
+      <c r="F53" s="27"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
-      <c r="J53" s="48"/>
+      <c r="J53" s="47"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="32" t="s">
+      <c r="A54" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="29" t="s">
+      <c r="D54" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E54" s="10"/>
-      <c r="F54" s="43"/>
+      <c r="F54" s="27"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
-      <c r="J54" s="48"/>
+      <c r="J54" s="47"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="32"/>
+      <c r="A55" s="36"/>
       <c r="B55" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="17"/>
-      <c r="D55" s="28"/>
+      <c r="D55" s="31"/>
       <c r="E55" s="10"/>
-      <c r="F55" s="43"/>
+      <c r="F55" s="27"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
-      <c r="J55" s="48"/>
+      <c r="J55" s="47"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="32"/>
+      <c r="A56" s="36"/>
       <c r="B56" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="17"/>
-      <c r="D56" s="28"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="10"/>
-      <c r="F56" s="43"/>
+      <c r="F56" s="27"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
-      <c r="J56" s="48"/>
+      <c r="J56" s="47"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="32"/>
+      <c r="A57" s="36"/>
       <c r="B57" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="30"/>
+      <c r="D57" s="33"/>
       <c r="E57" s="10"/>
-      <c r="F57" s="43"/>
+      <c r="F57" s="27"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
-      <c r="J57" s="48"/>
+      <c r="J57" s="47"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="36" t="s">
         <v>22</v>
       </c>
       <c r="B58" s="6" t="s">
@@ -2272,19 +2340,21 @@
       <c r="D58" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="43"/>
+      <c r="F58" s="27"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
-      <c r="I58" s="28" t="s">
+      <c r="I58" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="J58" s="48"/>
+      <c r="J58" s="50" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="32"/>
+      <c r="A59" s="36"/>
       <c r="B59" s="6" t="s">
         <v>12</v>
       </c>
@@ -2292,21 +2362,23 @@
       <c r="D59" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="31"/>
       <c r="F59" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="G59" s="27" t="s">
+      <c r="G59" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="27" t="s">
+      <c r="H59" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I59" s="28"/>
-      <c r="J59" s="48"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="50" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="32"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="6" t="s">
         <v>13</v>
       </c>
@@ -2314,17 +2386,17 @@
       <c r="D60" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="46" t="s">
+      <c r="E60" s="31"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="30" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="10"/>
-      <c r="I60" s="28"/>
-      <c r="J60" s="48"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="47"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="32"/>
+      <c r="A61" s="36"/>
       <c r="B61" s="6" t="s">
         <v>14</v>
       </c>
@@ -2332,195 +2404,199 @@
       <c r="D61" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="28"/>
+      <c r="E61" s="31"/>
       <c r="F61" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G61" s="27" t="s">
+      <c r="G61" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H61" s="27" t="s">
+      <c r="H61" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="I61" s="28"/>
-      <c r="J61" s="48"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="50" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="32"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
-      <c r="F62" s="43"/>
+      <c r="F62" s="27"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
-      <c r="J62" s="48"/>
+      <c r="J62" s="47"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="32"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
-      <c r="F63" s="43"/>
+      <c r="F63" s="27"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
-      <c r="J63" s="48"/>
+      <c r="J63" s="47"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="32"/>
+      <c r="A64" s="36"/>
       <c r="B64" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
-      <c r="F64" s="43"/>
+      <c r="F64" s="27"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
-      <c r="J64" s="48"/>
+      <c r="J64" s="47"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="32" t="s">
+      <c r="A65" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="11"/>
-      <c r="D65" s="29" t="s">
+      <c r="D65" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E65" s="28" t="s">
+      <c r="E65" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="F65" s="42" t="s">
+      <c r="F65" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="G65" s="31" t="s">
+      <c r="G65" s="43" t="s">
         <v>76</v>
       </c>
       <c r="H65" s="10"/>
-      <c r="I65" s="28" t="s">
+      <c r="I65" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="J65" s="48"/>
+      <c r="J65" s="47"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="32"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C66" s="17"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="43"/>
       <c r="H66" s="10"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="48"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="47"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="32"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="17"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="43"/>
       <c r="H67" s="10"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="48"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="47"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="32"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="5"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="31"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="43"/>
       <c r="H68" s="10"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="48"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="47"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="11"/>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="E69" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F69" s="43"/>
+      <c r="F69" s="27"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
-      <c r="I69" s="29" t="s">
+      <c r="I69" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="J69" s="48"/>
+      <c r="J69" s="50" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="32"/>
+      <c r="A70" s="36"/>
       <c r="B70" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C70" s="17"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="43"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="27"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="48"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="47"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="32"/>
+      <c r="A71" s="36"/>
       <c r="B71" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C71" s="17"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="43"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="27"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="48"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="47"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="32"/>
+      <c r="A72" s="36"/>
       <c r="B72" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="5"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="43"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="27"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="48"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="47"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="32" t="s">
+      <c r="A73" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="6" t="s">
@@ -2529,43 +2605,43 @@
       <c r="C73" s="11"/>
       <c r="D73" s="10"/>
       <c r="E73" s="10"/>
-      <c r="F73" s="43"/>
+      <c r="F73" s="27"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
-      <c r="J73" s="48"/>
+      <c r="J73" s="47"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="32"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C74" s="17"/>
       <c r="D74" s="10"/>
       <c r="E74" s="10"/>
-      <c r="F74" s="43"/>
+      <c r="F74" s="27"/>
       <c r="G74" s="10"/>
-      <c r="H74" s="27" t="s">
+      <c r="H74" s="26" t="s">
         <v>139</v>
       </c>
       <c r="I74" s="10"/>
-      <c r="J74" s="48"/>
+      <c r="J74" s="47"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="32"/>
+      <c r="A75" s="36"/>
       <c r="B75" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="46" t="s">
+      <c r="F75" s="27"/>
+      <c r="G75" s="30" t="s">
         <v>19</v>
       </c>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
-      <c r="J75" s="48"/>
+      <c r="J75" s="47"/>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="15" t="s">
@@ -2578,15 +2654,15 @@
       <c r="E76" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F76" s="43"/>
+      <c r="F76" s="27"/>
       <c r="G76" s="10"/>
-      <c r="H76" s="27" t="s">
+      <c r="H76" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="I76" s="26" t="s">
+      <c r="I76" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="J76" s="48"/>
+      <c r="J76" s="47"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="13" t="s">
@@ -2599,15 +2675,17 @@
       <c r="E77" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F77" s="43"/>
+      <c r="F77" s="27"/>
       <c r="G77" s="10"/>
-      <c r="H77" s="27" t="s">
+      <c r="H77" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="I77" s="27" t="s">
+      <c r="I77" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="J77" s="48"/>
+      <c r="J77" s="50" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="13" t="s">
@@ -2621,14 +2699,14 @@
       <c r="F78" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="G78" s="27" t="s">
+      <c r="G78" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H78" s="27" t="s">
+      <c r="H78" s="26" t="s">
         <v>132</v>
       </c>
       <c r="I78" s="10"/>
-      <c r="J78" s="48"/>
+      <c r="J78" s="47"/>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="13" t="s">
@@ -2644,14 +2722,16 @@
       <c r="F79" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="26" t="s">
         <v>54</v>
       </c>
       <c r="H79" s="10"/>
-      <c r="I79" s="26" t="s">
+      <c r="I79" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="J79" s="48"/>
+      <c r="J79" s="50" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="13" t="s">
@@ -2667,14 +2747,16 @@
       <c r="F80" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G80" s="27" t="s">
+      <c r="G80" s="26" t="s">
         <v>57</v>
       </c>
       <c r="H80" s="10"/>
-      <c r="I80" s="27" t="s">
+      <c r="I80" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="J80" s="48"/>
+      <c r="J80" s="50" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="13" t="s">
@@ -2686,12 +2768,14 @@
       <c r="F81" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="G81" s="27" t="s">
+      <c r="G81" s="26" t="s">
         <v>58</v>
       </c>
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
-      <c r="J81" s="48"/>
+      <c r="J81" s="50" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="13" t="s">
@@ -2707,14 +2791,14 @@
       <c r="F82" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G82" s="27" t="s">
+      <c r="G82" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H82" s="10"/>
-      <c r="I82" s="26" t="s">
+      <c r="I82" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="J82" s="48"/>
+      <c r="J82" s="47"/>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="13" t="s">
@@ -2723,11 +2807,11 @@
       <c r="B83" s="12"/>
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
-      <c r="F83" s="43"/>
+      <c r="F83" s="27"/>
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
-      <c r="J83" s="48"/>
+      <c r="J83" s="47"/>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="13" t="s">
@@ -2740,13 +2824,13 @@
       <c r="E84" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F84" s="43"/>
+      <c r="F84" s="27"/>
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
-      <c r="I84" s="26" t="s">
+      <c r="I84" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="J84" s="48"/>
+      <c r="J84" s="47"/>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="13" t="s">
@@ -2764,10 +2848,12 @@
       </c>
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
-      <c r="I85" s="25" t="s">
+      <c r="I85" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="J85" s="48"/>
+      <c r="J85" s="50" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="13" t="s">
@@ -2780,13 +2866,15 @@
       <c r="E86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F86" s="43"/>
+      <c r="F86" s="27"/>
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
-      <c r="I86" s="27" t="s">
+      <c r="I86" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="J86" s="48"/>
+      <c r="J86" s="50" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="13" t="s">
@@ -2795,11 +2883,11 @@
       <c r="B87" s="12"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
-      <c r="F87" s="43"/>
+      <c r="F87" s="27"/>
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
-      <c r="J87" s="48"/>
+      <c r="J87" s="47"/>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="13" t="s">
@@ -2812,13 +2900,15 @@
       <c r="E88" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F88" s="43"/>
+      <c r="F88" s="27"/>
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
-      <c r="I88" s="26" t="s">
+      <c r="I88" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="J88" s="48"/>
+      <c r="J88" s="50" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="16" t="s">
@@ -2829,14 +2919,14 @@
         <v>81</v>
       </c>
       <c r="E89" s="10"/>
-      <c r="F89" s="43"/>
+      <c r="F89" s="27"/>
       <c r="G89" s="10"/>
       <c r="H89" s="10"/>
       <c r="I89" s="10"/>
-      <c r="J89" s="48"/>
+      <c r="J89" s="47"/>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="36" t="s">
+      <c r="A90" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B90" s="6" t="s">
@@ -2850,15 +2940,15 @@
       <c r="F90" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G90" s="27" t="s">
+      <c r="G90" s="26" t="s">
         <v>24</v>
       </c>
       <c r="H90" s="10"/>
       <c r="I90" s="10"/>
-      <c r="J90" s="48"/>
+      <c r="J90" s="47"/>
     </row>
     <row r="91" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A91" s="37"/>
+      <c r="A91" s="35"/>
       <c r="B91" s="14" t="s">
         <v>25</v>
       </c>
@@ -2866,8 +2956,8 @@
       <c r="D91" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E91" s="24"/>
-      <c r="F91" s="44" t="s">
+      <c r="E91" s="23"/>
+      <c r="F91" s="28" t="s">
         <v>104</v>
       </c>
       <c r="G91" s="20" t="s">
@@ -2876,24 +2966,35 @@
       <c r="H91" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="I91" s="24"/>
-      <c r="J91" s="49"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="48"/>
     </row>
   </sheetData>
   <sortState ref="A2:A53">
     <sortCondition ref="A53"/>
   </sortState>
-  <mergeCells count="47">
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="I65:I68"/>
-    <mergeCell ref="I69:I72"/>
-    <mergeCell ref="J2:J91"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I26:I29"/>
-    <mergeCell ref="I30:I32"/>
+  <mergeCells count="46">
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G65:G68"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B29"/>
     <mergeCell ref="D65:D68"/>
     <mergeCell ref="A90:A91"/>
     <mergeCell ref="A69:A72"/>
@@ -2910,27 +3011,15 @@
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G65:G68"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="I65:I68"/>
+    <mergeCell ref="I69:I72"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I26:I29"/>
+    <mergeCell ref="I30:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>